<commit_message>
add -fPIC to compile lib
</commit_message>
<xml_diff>
--- a/doc/性能.xlsx
+++ b/doc/性能.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feiw\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feiw\source\repos\TensileLite\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1212AD3A-78DC-4F40-8006-A8111FC9DD50}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A34F3C-5178-4A30-A9C6-B25B56509DB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-12645" windowWidth="16440" windowHeight="28440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fp16" sheetId="5" r:id="rId1"/>
     <sheet name="fp32" sheetId="4" r:id="rId2"/>
+    <sheet name="phantom fp32" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="18">
   <si>
     <t>MT1</t>
   </si>
@@ -71,6 +72,24 @@
   <si>
     <t>rpk</t>
   </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>Tflops</t>
+  </si>
+  <si>
+    <t>M=512</t>
+  </si>
+  <si>
+    <t>N=512</t>
+  </si>
+  <si>
+    <t>M=480</t>
+  </si>
+  <si>
+    <t>N=480</t>
+  </si>
 </sst>
 </file>
 
@@ -88,7 +107,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -119,8 +138,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="16">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -337,11 +380,210 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -409,6 +651,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -427,7 +672,100 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -710,10 +1048,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAC527AE-D371-4150-9EA5-509D329EE9EA}">
-  <dimension ref="B4:N10"/>
+  <dimension ref="B4:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -724,37 +1062,37 @@
     <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="5" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B5" s="6"/>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="29">
+      <c r="D5" s="23">
         <v>758</v>
       </c>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="F5" s="29">
+      <c r="F5" s="23">
         <v>120</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="29">
+      <c r="H5" s="23">
         <f>D5*1024*F5/1000</f>
         <v>93143.039999999994</v>
       </c>
-      <c r="I5" s="23" t="s">
+      <c r="I5" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="24"/>
-      <c r="K5" s="25">
+      <c r="J5" s="25"/>
+      <c r="K5" s="26">
         <v>43885</v>
       </c>
-      <c r="L5" s="26"/>
-      <c r="M5" s="27">
+      <c r="L5" s="27"/>
+      <c r="M5" s="28">
         <v>43889</v>
       </c>
-      <c r="N5" s="28"/>
+      <c r="N5" s="29"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
@@ -971,6 +1309,17 @@
       <c r="N10" s="14">
         <f>M10/$H$5</f>
         <v>0.84311184174362364</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="E12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="1">
+        <v>64</v>
+      </c>
+      <c r="G12" s="1">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -989,12 +1338,1042 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF1495CF-1B82-46CC-A70C-A86AE3F67542}">
-  <dimension ref="A1"/>
+  <dimension ref="B4:N12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="16384" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B5" s="6"/>
+      <c r="C5" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="23">
+        <v>758</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="23">
+        <v>120</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="23">
+        <f>D5*1024*F5/1000</f>
+        <v>93143.039999999994</v>
+      </c>
+      <c r="I5" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="25"/>
+      <c r="K5" s="26">
+        <v>43885</v>
+      </c>
+      <c r="L5" s="27"/>
+      <c r="M5" s="28">
+        <v>43889</v>
+      </c>
+      <c r="N5" s="29"/>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="K6" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="M6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N6" s="8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B7" s="9">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2">
+        <v>960</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1024</v>
+      </c>
+      <c r="E7" s="2">
+        <v>1024</v>
+      </c>
+      <c r="F7" s="2">
+        <v>128</v>
+      </c>
+      <c r="G7" s="2">
+        <v>128</v>
+      </c>
+      <c r="H7" s="18">
+        <v>32</v>
+      </c>
+      <c r="I7" s="9">
+        <v>77492</v>
+      </c>
+      <c r="J7" s="10">
+        <f>I7/$H$5</f>
+        <v>0.83196769184256825</v>
+      </c>
+      <c r="K7" s="15">
+        <v>20470</v>
+      </c>
+      <c r="L7" s="3">
+        <f>K7/$H$5</f>
+        <v>0.21976950720096747</v>
+      </c>
+      <c r="M7" s="2">
+        <v>24070</v>
+      </c>
+      <c r="N7" s="10">
+        <f>M7/$H$5</f>
+        <v>0.25841973807167989</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B8" s="9">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1920</v>
+      </c>
+      <c r="D8" s="2">
+        <v>2048</v>
+      </c>
+      <c r="E8" s="2">
+        <v>2048</v>
+      </c>
+      <c r="F8" s="2">
+        <v>128</v>
+      </c>
+      <c r="G8" s="2">
+        <v>128</v>
+      </c>
+      <c r="H8" s="18">
+        <v>32</v>
+      </c>
+      <c r="I8" s="9">
+        <v>84796</v>
+      </c>
+      <c r="J8" s="10">
+        <f>I8/$H$5</f>
+        <v>0.91038471580914693</v>
+      </c>
+      <c r="K8" s="15">
+        <v>60700</v>
+      </c>
+      <c r="L8" s="3">
+        <f>K8/$H$5</f>
+        <v>0.65168583718117856</v>
+      </c>
+      <c r="M8" s="2">
+        <v>64730</v>
+      </c>
+      <c r="N8" s="10">
+        <f>M8/$H$5</f>
+        <v>0.6949526234058927</v>
+      </c>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="B9" s="9">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2">
+        <v>3840</v>
+      </c>
+      <c r="D9" s="2">
+        <v>4096</v>
+      </c>
+      <c r="E9" s="2">
+        <v>4096</v>
+      </c>
+      <c r="F9" s="2">
+        <v>128</v>
+      </c>
+      <c r="G9" s="2">
+        <v>128</v>
+      </c>
+      <c r="H9" s="18">
+        <v>32</v>
+      </c>
+      <c r="I9" s="9">
+        <v>88801</v>
+      </c>
+      <c r="J9" s="10">
+        <f>I9/$H$5</f>
+        <v>0.95338309765281448</v>
+      </c>
+      <c r="K9" s="15">
+        <v>65730</v>
+      </c>
+      <c r="L9" s="3">
+        <f>K9/$H$5</f>
+        <v>0.70568879864775735</v>
+      </c>
+      <c r="M9" s="2">
+        <v>73330</v>
+      </c>
+      <c r="N9" s="10">
+        <f>M9/$H$5</f>
+        <v>0.78728373048592792</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B10" s="11">
+        <v>4</v>
+      </c>
+      <c r="C10" s="12">
+        <v>7680</v>
+      </c>
+      <c r="D10" s="12">
+        <v>8192</v>
+      </c>
+      <c r="E10" s="12">
+        <v>8192</v>
+      </c>
+      <c r="F10" s="12">
+        <v>128</v>
+      </c>
+      <c r="G10" s="12">
+        <v>128</v>
+      </c>
+      <c r="H10" s="19">
+        <v>32</v>
+      </c>
+      <c r="I10" s="11">
+        <v>77492</v>
+      </c>
+      <c r="J10" s="14">
+        <f>I10/$H$5</f>
+        <v>0.83196769184256825</v>
+      </c>
+      <c r="K10" s="16">
+        <v>71390</v>
+      </c>
+      <c r="L10" s="13">
+        <f>K10/$H$5</f>
+        <v>0.76645555051671066</v>
+      </c>
+      <c r="M10" s="12">
+        <v>78530</v>
+      </c>
+      <c r="N10" s="14">
+        <f>M10/$H$5</f>
+        <v>0.84311184174362364</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.35">
+      <c r="E12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="1">
+        <v>64</v>
+      </c>
+      <c r="G12" s="1">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="K5:L5"/>
+    <mergeCell ref="M5:N5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"Arial"&amp;10&amp;K0078D7[AMD Official Use Only - Internal Distribution Only]&amp;1#</oddHeader>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D66D3AA-20DD-406F-9B75-9E00FD19467A}">
+  <dimension ref="B3:J30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H55" sqref="H55"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="16384" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="31"/>
+      <c r="C3" s="30" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="30">
+        <v>758</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="30">
+        <v>120</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="30">
+        <f>D3*256*F3/1000/1000</f>
+        <v>23.28576</v>
+      </c>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+    </row>
+    <row r="5" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+    </row>
+    <row r="6" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="57" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="49" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="53" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="44" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="59" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="61"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B8" s="54">
+        <v>1</v>
+      </c>
+      <c r="C8" s="40">
+        <v>512</v>
+      </c>
+      <c r="D8" s="41">
+        <v>512</v>
+      </c>
+      <c r="E8" s="41">
+        <v>512</v>
+      </c>
+      <c r="F8" s="41">
+        <v>32</v>
+      </c>
+      <c r="G8" s="41">
+        <v>128</v>
+      </c>
+      <c r="H8" s="50">
+        <v>32</v>
+      </c>
+      <c r="I8" s="46">
+        <v>5.0199999999999996</v>
+      </c>
+      <c r="J8" s="45">
+        <f>I8/$H$3</f>
+        <v>0.21558239885664027</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B9" s="55">
+        <v>2</v>
+      </c>
+      <c r="C9" s="42">
+        <v>512</v>
+      </c>
+      <c r="D9" s="33">
+        <v>1024</v>
+      </c>
+      <c r="E9" s="33">
+        <v>1024</v>
+      </c>
+      <c r="F9" s="33">
+        <v>32</v>
+      </c>
+      <c r="G9" s="33">
+        <v>128</v>
+      </c>
+      <c r="H9" s="51">
+        <v>32</v>
+      </c>
+      <c r="I9" s="47">
+        <v>7.45</v>
+      </c>
+      <c r="J9" s="34">
+        <f t="shared" ref="J9:J30" si="0">I9/$H$3</f>
+        <v>0.31993802220756379</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="55">
+        <v>3</v>
+      </c>
+      <c r="C10" s="42">
+        <v>512</v>
+      </c>
+      <c r="D10" s="33">
+        <v>2048</v>
+      </c>
+      <c r="E10" s="33">
+        <v>2048</v>
+      </c>
+      <c r="F10" s="33">
+        <v>32</v>
+      </c>
+      <c r="G10" s="33">
+        <v>128</v>
+      </c>
+      <c r="H10" s="51">
+        <v>32</v>
+      </c>
+      <c r="I10" s="47">
+        <v>11.06</v>
+      </c>
+      <c r="J10" s="34">
+        <f t="shared" si="0"/>
+        <v>0.47496839270008795</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="55">
+        <v>4</v>
+      </c>
+      <c r="C11" s="42">
+        <v>512</v>
+      </c>
+      <c r="D11" s="33">
+        <v>4096</v>
+      </c>
+      <c r="E11" s="33">
+        <v>4096</v>
+      </c>
+      <c r="F11" s="33">
+        <v>32</v>
+      </c>
+      <c r="G11" s="33">
+        <v>128</v>
+      </c>
+      <c r="H11" s="51">
+        <v>32</v>
+      </c>
+      <c r="I11" s="47">
+        <v>13.61</v>
+      </c>
+      <c r="J11" s="34">
+        <f t="shared" si="0"/>
+        <v>0.58447738016710638</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="56">
+        <v>5</v>
+      </c>
+      <c r="C12" s="43">
+        <v>512</v>
+      </c>
+      <c r="D12" s="35">
+        <v>8192</v>
+      </c>
+      <c r="E12" s="35">
+        <v>8192</v>
+      </c>
+      <c r="F12" s="35">
+        <v>32</v>
+      </c>
+      <c r="G12" s="35">
+        <v>128</v>
+      </c>
+      <c r="H12" s="52">
+        <v>32</v>
+      </c>
+      <c r="I12" s="48">
+        <v>14.83</v>
+      </c>
+      <c r="J12" s="36">
+        <f t="shared" si="0"/>
+        <v>0.63686991534740545</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="60"/>
+      <c r="D13" s="60"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="60"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="60"/>
+      <c r="I13" s="60"/>
+      <c r="J13" s="61"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B14" s="54">
+        <v>6</v>
+      </c>
+      <c r="C14" s="40">
+        <v>512</v>
+      </c>
+      <c r="D14" s="41">
+        <v>512</v>
+      </c>
+      <c r="E14" s="41">
+        <v>512</v>
+      </c>
+      <c r="F14" s="41">
+        <v>128</v>
+      </c>
+      <c r="G14" s="41">
+        <v>32</v>
+      </c>
+      <c r="H14" s="50">
+        <v>32</v>
+      </c>
+      <c r="I14" s="46">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="J14" s="45">
+        <f t="shared" si="0"/>
+        <v>0.21386461081794197</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B15" s="55">
+        <v>7</v>
+      </c>
+      <c r="C15" s="42">
+        <v>1024</v>
+      </c>
+      <c r="D15" s="33">
+        <v>512</v>
+      </c>
+      <c r="E15" s="33">
+        <v>1024</v>
+      </c>
+      <c r="F15" s="33">
+        <v>128</v>
+      </c>
+      <c r="G15" s="33">
+        <v>32</v>
+      </c>
+      <c r="H15" s="51">
+        <v>32</v>
+      </c>
+      <c r="I15" s="47">
+        <v>7.53</v>
+      </c>
+      <c r="J15" s="34">
+        <f t="shared" si="0"/>
+        <v>0.32337359828496043</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B16" s="55">
+        <v>8</v>
+      </c>
+      <c r="C16" s="42">
+        <v>2048</v>
+      </c>
+      <c r="D16" s="33">
+        <v>512</v>
+      </c>
+      <c r="E16" s="33">
+        <v>2048</v>
+      </c>
+      <c r="F16" s="33">
+        <v>128</v>
+      </c>
+      <c r="G16" s="33">
+        <v>32</v>
+      </c>
+      <c r="H16" s="51">
+        <v>32</v>
+      </c>
+      <c r="I16" s="47">
+        <v>11.16</v>
+      </c>
+      <c r="J16" s="34">
+        <f t="shared" si="0"/>
+        <v>0.47926286279683378</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B17" s="55">
+        <v>9</v>
+      </c>
+      <c r="C17" s="42">
+        <v>4096</v>
+      </c>
+      <c r="D17" s="33">
+        <v>512</v>
+      </c>
+      <c r="E17" s="33">
+        <v>4096</v>
+      </c>
+      <c r="F17" s="33">
+        <v>128</v>
+      </c>
+      <c r="G17" s="33">
+        <v>32</v>
+      </c>
+      <c r="H17" s="51">
+        <v>32</v>
+      </c>
+      <c r="I17" s="47">
+        <v>13.8</v>
+      </c>
+      <c r="J17" s="34">
+        <f t="shared" si="0"/>
+        <v>0.59263687335092352</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="56">
+        <v>10</v>
+      </c>
+      <c r="C18" s="43">
+        <v>8192</v>
+      </c>
+      <c r="D18" s="35">
+        <v>512</v>
+      </c>
+      <c r="E18" s="35">
+        <v>8192</v>
+      </c>
+      <c r="F18" s="35">
+        <v>128</v>
+      </c>
+      <c r="G18" s="35">
+        <v>32</v>
+      </c>
+      <c r="H18" s="52">
+        <v>32</v>
+      </c>
+      <c r="I18" s="48">
+        <v>14.48</v>
+      </c>
+      <c r="J18" s="36">
+        <f t="shared" si="0"/>
+        <v>0.62183927000879513</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="59" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="60"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="60"/>
+      <c r="H19" s="60"/>
+      <c r="I19" s="60"/>
+      <c r="J19" s="61"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B20" s="54">
+        <v>11</v>
+      </c>
+      <c r="C20" s="40">
+        <v>480</v>
+      </c>
+      <c r="D20" s="41">
+        <v>512</v>
+      </c>
+      <c r="E20" s="41">
+        <v>512</v>
+      </c>
+      <c r="F20" s="41">
+        <v>32</v>
+      </c>
+      <c r="G20" s="41">
+        <v>128</v>
+      </c>
+      <c r="H20" s="50">
+        <v>32</v>
+      </c>
+      <c r="I20" s="46">
+        <v>4.47</v>
+      </c>
+      <c r="J20" s="45">
+        <f t="shared" si="0"/>
+        <v>0.19196281332453824</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B21" s="55">
+        <v>12</v>
+      </c>
+      <c r="C21" s="42">
+        <v>480</v>
+      </c>
+      <c r="D21" s="33">
+        <v>1024</v>
+      </c>
+      <c r="E21" s="33">
+        <v>1024</v>
+      </c>
+      <c r="F21" s="33">
+        <v>32</v>
+      </c>
+      <c r="G21" s="33">
+        <v>128</v>
+      </c>
+      <c r="H21" s="51">
+        <v>32</v>
+      </c>
+      <c r="I21" s="47">
+        <v>9.75</v>
+      </c>
+      <c r="J21" s="34">
+        <f t="shared" si="0"/>
+        <v>0.41871083443271767</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B22" s="55">
+        <v>13</v>
+      </c>
+      <c r="C22" s="42">
+        <v>480</v>
+      </c>
+      <c r="D22" s="33">
+        <v>2048</v>
+      </c>
+      <c r="E22" s="33">
+        <v>2048</v>
+      </c>
+      <c r="F22" s="33">
+        <v>32</v>
+      </c>
+      <c r="G22" s="33">
+        <v>128</v>
+      </c>
+      <c r="H22" s="51">
+        <v>32</v>
+      </c>
+      <c r="I22" s="47">
+        <v>12.46</v>
+      </c>
+      <c r="J22" s="34">
+        <f t="shared" si="0"/>
+        <v>0.53509097405452954</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B23" s="55">
+        <v>14</v>
+      </c>
+      <c r="C23" s="42">
+        <v>480</v>
+      </c>
+      <c r="D23" s="33">
+        <v>4096</v>
+      </c>
+      <c r="E23" s="33">
+        <v>4096</v>
+      </c>
+      <c r="F23" s="33">
+        <v>32</v>
+      </c>
+      <c r="G23" s="33">
+        <v>128</v>
+      </c>
+      <c r="H23" s="51">
+        <v>32</v>
+      </c>
+      <c r="I23" s="47">
+        <v>14.45</v>
+      </c>
+      <c r="J23" s="34">
+        <f t="shared" si="0"/>
+        <v>0.62055092897977127</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B24" s="56">
+        <v>15</v>
+      </c>
+      <c r="C24" s="43">
+        <v>480</v>
+      </c>
+      <c r="D24" s="35">
+        <v>8192</v>
+      </c>
+      <c r="E24" s="35">
+        <v>8192</v>
+      </c>
+      <c r="F24" s="35">
+        <v>32</v>
+      </c>
+      <c r="G24" s="35">
+        <v>128</v>
+      </c>
+      <c r="H24" s="52">
+        <v>32</v>
+      </c>
+      <c r="I24" s="48">
+        <v>15.3</v>
+      </c>
+      <c r="J24" s="36">
+        <f t="shared" si="0"/>
+        <v>0.65705392480211089</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B25" s="59" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="60"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="60"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="60"/>
+      <c r="H25" s="60"/>
+      <c r="I25" s="60"/>
+      <c r="J25" s="61"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B26" s="58">
+        <v>16</v>
+      </c>
+      <c r="C26" s="40">
+        <v>512</v>
+      </c>
+      <c r="D26" s="41">
+        <v>480</v>
+      </c>
+      <c r="E26" s="41">
+        <v>512</v>
+      </c>
+      <c r="F26" s="41">
+        <v>128</v>
+      </c>
+      <c r="G26" s="41">
+        <v>32</v>
+      </c>
+      <c r="H26" s="50">
+        <v>32</v>
+      </c>
+      <c r="I26" s="46">
+        <v>4.71</v>
+      </c>
+      <c r="J26" s="45">
+        <f t="shared" si="0"/>
+        <v>0.20226954155672824</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B27" s="37">
+        <v>17</v>
+      </c>
+      <c r="C27" s="42">
+        <v>1024</v>
+      </c>
+      <c r="D27" s="33">
+        <v>480</v>
+      </c>
+      <c r="E27" s="33">
+        <v>1024</v>
+      </c>
+      <c r="F27" s="33">
+        <v>128</v>
+      </c>
+      <c r="G27" s="33">
+        <v>32</v>
+      </c>
+      <c r="H27" s="51">
+        <v>32</v>
+      </c>
+      <c r="I27" s="47">
+        <v>10.26</v>
+      </c>
+      <c r="J27" s="34">
+        <f t="shared" si="0"/>
+        <v>0.44061263192612138</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B28" s="37">
+        <v>18</v>
+      </c>
+      <c r="C28" s="42">
+        <v>2048</v>
+      </c>
+      <c r="D28" s="33">
+        <v>480</v>
+      </c>
+      <c r="E28" s="33">
+        <v>2048</v>
+      </c>
+      <c r="F28" s="33">
+        <v>128</v>
+      </c>
+      <c r="G28" s="33">
+        <v>32</v>
+      </c>
+      <c r="H28" s="51">
+        <v>32</v>
+      </c>
+      <c r="I28" s="47">
+        <v>13.19</v>
+      </c>
+      <c r="J28" s="34">
+        <f t="shared" si="0"/>
+        <v>0.56644060576077393</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B29" s="37">
+        <v>19</v>
+      </c>
+      <c r="C29" s="42">
+        <v>4096</v>
+      </c>
+      <c r="D29" s="33">
+        <v>480</v>
+      </c>
+      <c r="E29" s="33">
+        <v>4096</v>
+      </c>
+      <c r="F29" s="33">
+        <v>128</v>
+      </c>
+      <c r="G29" s="33">
+        <v>32</v>
+      </c>
+      <c r="H29" s="51">
+        <v>32</v>
+      </c>
+      <c r="I29" s="47">
+        <v>14.83</v>
+      </c>
+      <c r="J29" s="34">
+        <f t="shared" si="0"/>
+        <v>0.63686991534740545</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B30" s="38">
+        <v>20</v>
+      </c>
+      <c r="C30" s="43">
+        <v>8192</v>
+      </c>
+      <c r="D30" s="35">
+        <v>480</v>
+      </c>
+      <c r="E30" s="35">
+        <v>8192</v>
+      </c>
+      <c r="F30" s="35">
+        <v>128</v>
+      </c>
+      <c r="G30" s="35">
+        <v>32</v>
+      </c>
+      <c r="H30" s="52">
+        <v>32</v>
+      </c>
+      <c r="I30" s="48">
+        <v>14.43</v>
+      </c>
+      <c r="J30" s="36">
+        <f t="shared" si="0"/>
+        <v>0.61969203496042213</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="B25:J25"/>
+    <mergeCell ref="B19:J19"/>
+    <mergeCell ref="B13:J13"/>
+    <mergeCell ref="B7:J7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter>

</xml_diff>

<commit_message>
add bf16 support for phantom size
</commit_message>
<xml_diff>
--- a/doc/性能.xlsx
+++ b/doc/性能.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feiw\source\repos\TensileLite\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A34F3C-5178-4A30-A9C6-B25B56509DB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFAB5739-094C-43D1-8F93-5FFCA431942D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="-12645" windowWidth="16440" windowHeight="28440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16320" yWindow="-12645" windowWidth="16440" windowHeight="28440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fp16" sheetId="5" r:id="rId1"/>
     <sheet name="fp32" sheetId="4" r:id="rId2"/>
     <sheet name="phantom fp32" sheetId="6" r:id="rId3"/>
+    <sheet name="phantom bf16" sheetId="7" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="18">
   <si>
     <t>MT1</t>
   </si>
@@ -583,7 +584,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -654,6 +655,93 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -672,91 +760,7 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="9" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="9" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="9" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1081,18 +1085,18 @@
         <f>D5*1024*F5/1000</f>
         <v>93143.039999999994</v>
       </c>
-      <c r="I5" s="24" t="s">
+      <c r="I5" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="25"/>
-      <c r="K5" s="26">
+      <c r="J5" s="54"/>
+      <c r="K5" s="55">
         <v>43885</v>
       </c>
-      <c r="L5" s="27"/>
-      <c r="M5" s="28">
+      <c r="L5" s="56"/>
+      <c r="M5" s="57">
         <v>43889</v>
       </c>
-      <c r="N5" s="29"/>
+      <c r="N5" s="58"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
@@ -1371,18 +1375,18 @@
         <f>D5*1024*F5/1000</f>
         <v>93143.039999999994</v>
       </c>
-      <c r="I5" s="24" t="s">
+      <c r="I5" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="25"/>
-      <c r="K5" s="26">
+      <c r="J5" s="54"/>
+      <c r="K5" s="55">
         <v>43885</v>
       </c>
-      <c r="L5" s="27"/>
-      <c r="M5" s="28">
+      <c r="L5" s="56"/>
+      <c r="M5" s="57">
         <v>43889</v>
       </c>
-      <c r="N5" s="29"/>
+      <c r="N5" s="58"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
@@ -1630,8 +1634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D66D3AA-20DD-406F-9B75-9E00FD19467A}">
   <dimension ref="B3:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H55" sqref="H55"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1640,728 +1644,728 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B3" s="31"/>
-      <c r="C3" s="30" t="s">
+      <c r="B3" s="25"/>
+      <c r="C3" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="30">
+      <c r="D3" s="24">
         <v>758</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="30">
+      <c r="F3" s="24">
         <v>120</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="30">
+      <c r="H3" s="24">
         <f>D3*256*F3/1000/1000</f>
         <v>23.28576</v>
       </c>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
     </row>
     <row r="5" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B5" s="31"/>
-      <c r="C5" s="31"/>
-      <c r="D5" s="31"/>
-      <c r="E5" s="31"/>
-      <c r="F5" s="31"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="31"/>
-      <c r="I5" s="31"/>
-      <c r="J5" s="31"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
     </row>
     <row r="6" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="51" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="39" t="s">
+      <c r="C6" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="39" t="s">
+      <c r="D6" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="39" t="s">
+      <c r="E6" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="39" t="s">
+      <c r="F6" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="G6" s="39" t="s">
+      <c r="G6" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="H6" s="49" t="s">
+      <c r="H6" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="53" t="s">
+      <c r="I6" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="44" t="s">
+      <c r="J6" s="38" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="60"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="61"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="61"/>
+      <c r="J7" s="62"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B8" s="54">
+      <c r="B8" s="48">
         <v>1</v>
       </c>
-      <c r="C8" s="40">
-        <v>512</v>
-      </c>
-      <c r="D8" s="41">
-        <v>512</v>
-      </c>
-      <c r="E8" s="41">
-        <v>512</v>
-      </c>
-      <c r="F8" s="41">
-        <v>32</v>
-      </c>
-      <c r="G8" s="41">
-        <v>128</v>
-      </c>
-      <c r="H8" s="50">
-        <v>32</v>
-      </c>
-      <c r="I8" s="46">
+      <c r="C8" s="34">
+        <v>512</v>
+      </c>
+      <c r="D8" s="35">
+        <v>512</v>
+      </c>
+      <c r="E8" s="35">
+        <v>512</v>
+      </c>
+      <c r="F8" s="35">
+        <v>32</v>
+      </c>
+      <c r="G8" s="35">
+        <v>128</v>
+      </c>
+      <c r="H8" s="44">
+        <v>32</v>
+      </c>
+      <c r="I8" s="40">
         <v>5.0199999999999996</v>
       </c>
-      <c r="J8" s="45">
+      <c r="J8" s="39">
         <f>I8/$H$3</f>
         <v>0.21558239885664027</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B9" s="55">
+      <c r="B9" s="49">
         <v>2</v>
       </c>
-      <c r="C9" s="42">
-        <v>512</v>
-      </c>
-      <c r="D9" s="33">
+      <c r="C9" s="36">
+        <v>512</v>
+      </c>
+      <c r="D9" s="27">
         <v>1024</v>
       </c>
-      <c r="E9" s="33">
+      <c r="E9" s="27">
         <v>1024</v>
       </c>
-      <c r="F9" s="33">
-        <v>32</v>
-      </c>
-      <c r="G9" s="33">
-        <v>128</v>
-      </c>
-      <c r="H9" s="51">
-        <v>32</v>
-      </c>
-      <c r="I9" s="47">
+      <c r="F9" s="27">
+        <v>32</v>
+      </c>
+      <c r="G9" s="27">
+        <v>128</v>
+      </c>
+      <c r="H9" s="45">
+        <v>32</v>
+      </c>
+      <c r="I9" s="41">
         <v>7.45</v>
       </c>
-      <c r="J9" s="34">
+      <c r="J9" s="28">
         <f t="shared" ref="J9:J30" si="0">I9/$H$3</f>
         <v>0.31993802220756379</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B10" s="55">
+      <c r="B10" s="49">
         <v>3</v>
       </c>
-      <c r="C10" s="42">
-        <v>512</v>
-      </c>
-      <c r="D10" s="33">
+      <c r="C10" s="36">
+        <v>512</v>
+      </c>
+      <c r="D10" s="27">
         <v>2048</v>
       </c>
-      <c r="E10" s="33">
+      <c r="E10" s="27">
         <v>2048</v>
       </c>
-      <c r="F10" s="33">
-        <v>32</v>
-      </c>
-      <c r="G10" s="33">
-        <v>128</v>
-      </c>
-      <c r="H10" s="51">
-        <v>32</v>
-      </c>
-      <c r="I10" s="47">
+      <c r="F10" s="27">
+        <v>32</v>
+      </c>
+      <c r="G10" s="27">
+        <v>128</v>
+      </c>
+      <c r="H10" s="45">
+        <v>32</v>
+      </c>
+      <c r="I10" s="41">
         <v>11.06</v>
       </c>
-      <c r="J10" s="34">
+      <c r="J10" s="28">
         <f t="shared" si="0"/>
         <v>0.47496839270008795</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B11" s="55">
+      <c r="B11" s="49">
         <v>4</v>
       </c>
-      <c r="C11" s="42">
-        <v>512</v>
-      </c>
-      <c r="D11" s="33">
+      <c r="C11" s="36">
+        <v>512</v>
+      </c>
+      <c r="D11" s="27">
         <v>4096</v>
       </c>
-      <c r="E11" s="33">
+      <c r="E11" s="27">
         <v>4096</v>
       </c>
-      <c r="F11" s="33">
-        <v>32</v>
-      </c>
-      <c r="G11" s="33">
-        <v>128</v>
-      </c>
-      <c r="H11" s="51">
-        <v>32</v>
-      </c>
-      <c r="I11" s="47">
+      <c r="F11" s="27">
+        <v>32</v>
+      </c>
+      <c r="G11" s="27">
+        <v>128</v>
+      </c>
+      <c r="H11" s="45">
+        <v>32</v>
+      </c>
+      <c r="I11" s="41">
         <v>13.61</v>
       </c>
-      <c r="J11" s="34">
+      <c r="J11" s="28">
         <f t="shared" si="0"/>
         <v>0.58447738016710638</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B12" s="56">
+      <c r="B12" s="50">
         <v>5</v>
       </c>
-      <c r="C12" s="43">
-        <v>512</v>
-      </c>
-      <c r="D12" s="35">
+      <c r="C12" s="37">
+        <v>512</v>
+      </c>
+      <c r="D12" s="29">
         <v>8192</v>
       </c>
-      <c r="E12" s="35">
+      <c r="E12" s="29">
         <v>8192</v>
       </c>
-      <c r="F12" s="35">
-        <v>32</v>
-      </c>
-      <c r="G12" s="35">
-        <v>128</v>
-      </c>
-      <c r="H12" s="52">
-        <v>32</v>
-      </c>
-      <c r="I12" s="48">
+      <c r="F12" s="29">
+        <v>32</v>
+      </c>
+      <c r="G12" s="29">
+        <v>128</v>
+      </c>
+      <c r="H12" s="46">
+        <v>32</v>
+      </c>
+      <c r="I12" s="42">
         <v>14.83</v>
       </c>
-      <c r="J12" s="36">
+      <c r="J12" s="30">
         <f t="shared" si="0"/>
         <v>0.63686991534740545</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="59" t="s">
+      <c r="B13" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="60"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="60"/>
-      <c r="F13" s="60"/>
-      <c r="G13" s="60"/>
-      <c r="H13" s="60"/>
-      <c r="I13" s="60"/>
-      <c r="J13" s="61"/>
+      <c r="C13" s="61"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="61"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="61"/>
+      <c r="J13" s="62"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B14" s="54">
+      <c r="B14" s="48">
         <v>6</v>
       </c>
-      <c r="C14" s="40">
-        <v>512</v>
-      </c>
-      <c r="D14" s="41">
-        <v>512</v>
-      </c>
-      <c r="E14" s="41">
-        <v>512</v>
-      </c>
-      <c r="F14" s="41">
-        <v>128</v>
-      </c>
-      <c r="G14" s="41">
-        <v>32</v>
-      </c>
-      <c r="H14" s="50">
-        <v>32</v>
-      </c>
-      <c r="I14" s="46">
+      <c r="C14" s="34">
+        <v>512</v>
+      </c>
+      <c r="D14" s="35">
+        <v>512</v>
+      </c>
+      <c r="E14" s="35">
+        <v>512</v>
+      </c>
+      <c r="F14" s="35">
+        <v>128</v>
+      </c>
+      <c r="G14" s="35">
+        <v>32</v>
+      </c>
+      <c r="H14" s="44">
+        <v>32</v>
+      </c>
+      <c r="I14" s="40">
         <v>4.9800000000000004</v>
       </c>
-      <c r="J14" s="45">
+      <c r="J14" s="39">
         <f t="shared" si="0"/>
         <v>0.21386461081794197</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B15" s="55">
+      <c r="B15" s="49">
         <v>7</v>
       </c>
-      <c r="C15" s="42">
+      <c r="C15" s="36">
         <v>1024</v>
       </c>
-      <c r="D15" s="33">
-        <v>512</v>
-      </c>
-      <c r="E15" s="33">
+      <c r="D15" s="27">
+        <v>512</v>
+      </c>
+      <c r="E15" s="27">
         <v>1024</v>
       </c>
-      <c r="F15" s="33">
-        <v>128</v>
-      </c>
-      <c r="G15" s="33">
-        <v>32</v>
-      </c>
-      <c r="H15" s="51">
-        <v>32</v>
-      </c>
-      <c r="I15" s="47">
+      <c r="F15" s="27">
+        <v>128</v>
+      </c>
+      <c r="G15" s="27">
+        <v>32</v>
+      </c>
+      <c r="H15" s="45">
+        <v>32</v>
+      </c>
+      <c r="I15" s="41">
         <v>7.53</v>
       </c>
-      <c r="J15" s="34">
+      <c r="J15" s="28">
         <f t="shared" si="0"/>
         <v>0.32337359828496043</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B16" s="55">
+      <c r="B16" s="49">
         <v>8</v>
       </c>
-      <c r="C16" s="42">
+      <c r="C16" s="36">
         <v>2048</v>
       </c>
-      <c r="D16" s="33">
-        <v>512</v>
-      </c>
-      <c r="E16" s="33">
+      <c r="D16" s="27">
+        <v>512</v>
+      </c>
+      <c r="E16" s="27">
         <v>2048</v>
       </c>
-      <c r="F16" s="33">
-        <v>128</v>
-      </c>
-      <c r="G16" s="33">
-        <v>32</v>
-      </c>
-      <c r="H16" s="51">
-        <v>32</v>
-      </c>
-      <c r="I16" s="47">
+      <c r="F16" s="27">
+        <v>128</v>
+      </c>
+      <c r="G16" s="27">
+        <v>32</v>
+      </c>
+      <c r="H16" s="45">
+        <v>32</v>
+      </c>
+      <c r="I16" s="41">
         <v>11.16</v>
       </c>
-      <c r="J16" s="34">
+      <c r="J16" s="28">
         <f t="shared" si="0"/>
         <v>0.47926286279683378</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B17" s="55">
+      <c r="B17" s="49">
         <v>9</v>
       </c>
-      <c r="C17" s="42">
+      <c r="C17" s="36">
         <v>4096</v>
       </c>
-      <c r="D17" s="33">
-        <v>512</v>
-      </c>
-      <c r="E17" s="33">
+      <c r="D17" s="27">
+        <v>512</v>
+      </c>
+      <c r="E17" s="27">
         <v>4096</v>
       </c>
-      <c r="F17" s="33">
-        <v>128</v>
-      </c>
-      <c r="G17" s="33">
-        <v>32</v>
-      </c>
-      <c r="H17" s="51">
-        <v>32</v>
-      </c>
-      <c r="I17" s="47">
+      <c r="F17" s="27">
+        <v>128</v>
+      </c>
+      <c r="G17" s="27">
+        <v>32</v>
+      </c>
+      <c r="H17" s="45">
+        <v>32</v>
+      </c>
+      <c r="I17" s="41">
         <v>13.8</v>
       </c>
-      <c r="J17" s="34">
+      <c r="J17" s="28">
         <f t="shared" si="0"/>
         <v>0.59263687335092352</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B18" s="56">
+      <c r="B18" s="50">
         <v>10</v>
       </c>
-      <c r="C18" s="43">
+      <c r="C18" s="37">
         <v>8192</v>
       </c>
-      <c r="D18" s="35">
-        <v>512</v>
-      </c>
-      <c r="E18" s="35">
+      <c r="D18" s="29">
+        <v>512</v>
+      </c>
+      <c r="E18" s="29">
         <v>8192</v>
       </c>
-      <c r="F18" s="35">
-        <v>128</v>
-      </c>
-      <c r="G18" s="35">
-        <v>32</v>
-      </c>
-      <c r="H18" s="52">
-        <v>32</v>
-      </c>
-      <c r="I18" s="48">
+      <c r="F18" s="29">
+        <v>128</v>
+      </c>
+      <c r="G18" s="29">
+        <v>32</v>
+      </c>
+      <c r="H18" s="46">
+        <v>32</v>
+      </c>
+      <c r="I18" s="42">
         <v>14.48</v>
       </c>
-      <c r="J18" s="36">
+      <c r="J18" s="30">
         <f t="shared" si="0"/>
         <v>0.62183927000879513</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="59" t="s">
+      <c r="B19" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="60"/>
-      <c r="H19" s="60"/>
-      <c r="I19" s="60"/>
-      <c r="J19" s="61"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="61"/>
+      <c r="H19" s="61"/>
+      <c r="I19" s="61"/>
+      <c r="J19" s="62"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B20" s="54">
+      <c r="B20" s="48">
         <v>11</v>
       </c>
-      <c r="C20" s="40">
+      <c r="C20" s="34">
         <v>480</v>
       </c>
-      <c r="D20" s="41">
-        <v>512</v>
-      </c>
-      <c r="E20" s="41">
-        <v>512</v>
-      </c>
-      <c r="F20" s="41">
-        <v>32</v>
-      </c>
-      <c r="G20" s="41">
-        <v>128</v>
-      </c>
-      <c r="H20" s="50">
-        <v>32</v>
-      </c>
-      <c r="I20" s="46">
+      <c r="D20" s="35">
+        <v>512</v>
+      </c>
+      <c r="E20" s="35">
+        <v>512</v>
+      </c>
+      <c r="F20" s="35">
+        <v>32</v>
+      </c>
+      <c r="G20" s="35">
+        <v>128</v>
+      </c>
+      <c r="H20" s="44">
+        <v>32</v>
+      </c>
+      <c r="I20" s="40">
         <v>4.47</v>
       </c>
-      <c r="J20" s="45">
+      <c r="J20" s="39">
         <f t="shared" si="0"/>
         <v>0.19196281332453824</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B21" s="55">
+      <c r="B21" s="49">
         <v>12</v>
       </c>
-      <c r="C21" s="42">
+      <c r="C21" s="36">
         <v>480</v>
       </c>
-      <c r="D21" s="33">
+      <c r="D21" s="27">
         <v>1024</v>
       </c>
-      <c r="E21" s="33">
+      <c r="E21" s="27">
         <v>1024</v>
       </c>
-      <c r="F21" s="33">
-        <v>32</v>
-      </c>
-      <c r="G21" s="33">
-        <v>128</v>
-      </c>
-      <c r="H21" s="51">
-        <v>32</v>
-      </c>
-      <c r="I21" s="47">
+      <c r="F21" s="27">
+        <v>32</v>
+      </c>
+      <c r="G21" s="27">
+        <v>128</v>
+      </c>
+      <c r="H21" s="45">
+        <v>32</v>
+      </c>
+      <c r="I21" s="41">
         <v>9.75</v>
       </c>
-      <c r="J21" s="34">
+      <c r="J21" s="28">
         <f t="shared" si="0"/>
         <v>0.41871083443271767</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B22" s="55">
+      <c r="B22" s="49">
         <v>13</v>
       </c>
-      <c r="C22" s="42">
+      <c r="C22" s="36">
         <v>480</v>
       </c>
-      <c r="D22" s="33">
+      <c r="D22" s="27">
         <v>2048</v>
       </c>
-      <c r="E22" s="33">
+      <c r="E22" s="27">
         <v>2048</v>
       </c>
-      <c r="F22" s="33">
-        <v>32</v>
-      </c>
-      <c r="G22" s="33">
-        <v>128</v>
-      </c>
-      <c r="H22" s="51">
-        <v>32</v>
-      </c>
-      <c r="I22" s="47">
+      <c r="F22" s="27">
+        <v>32</v>
+      </c>
+      <c r="G22" s="27">
+        <v>128</v>
+      </c>
+      <c r="H22" s="45">
+        <v>32</v>
+      </c>
+      <c r="I22" s="41">
         <v>12.46</v>
       </c>
-      <c r="J22" s="34">
+      <c r="J22" s="28">
         <f t="shared" si="0"/>
         <v>0.53509097405452954</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B23" s="55">
+      <c r="B23" s="49">
         <v>14</v>
       </c>
-      <c r="C23" s="42">
+      <c r="C23" s="36">
         <v>480</v>
       </c>
-      <c r="D23" s="33">
+      <c r="D23" s="27">
         <v>4096</v>
       </c>
-      <c r="E23" s="33">
+      <c r="E23" s="27">
         <v>4096</v>
       </c>
-      <c r="F23" s="33">
-        <v>32</v>
-      </c>
-      <c r="G23" s="33">
-        <v>128</v>
-      </c>
-      <c r="H23" s="51">
-        <v>32</v>
-      </c>
-      <c r="I23" s="47">
+      <c r="F23" s="27">
+        <v>32</v>
+      </c>
+      <c r="G23" s="27">
+        <v>128</v>
+      </c>
+      <c r="H23" s="45">
+        <v>32</v>
+      </c>
+      <c r="I23" s="41">
         <v>14.45</v>
       </c>
-      <c r="J23" s="34">
+      <c r="J23" s="28">
         <f t="shared" si="0"/>
         <v>0.62055092897977127</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B24" s="56">
+      <c r="B24" s="50">
         <v>15</v>
       </c>
-      <c r="C24" s="43">
+      <c r="C24" s="37">
         <v>480</v>
       </c>
-      <c r="D24" s="35">
+      <c r="D24" s="29">
         <v>8192</v>
       </c>
-      <c r="E24" s="35">
+      <c r="E24" s="29">
         <v>8192</v>
       </c>
-      <c r="F24" s="35">
-        <v>32</v>
-      </c>
-      <c r="G24" s="35">
-        <v>128</v>
-      </c>
-      <c r="H24" s="52">
-        <v>32</v>
-      </c>
-      <c r="I24" s="48">
+      <c r="F24" s="29">
+        <v>32</v>
+      </c>
+      <c r="G24" s="29">
+        <v>128</v>
+      </c>
+      <c r="H24" s="46">
+        <v>32</v>
+      </c>
+      <c r="I24" s="42">
         <v>15.3</v>
       </c>
-      <c r="J24" s="36">
+      <c r="J24" s="30">
         <f t="shared" si="0"/>
         <v>0.65705392480211089</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="59" t="s">
+      <c r="B25" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="60"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="60"/>
-      <c r="F25" s="60"/>
-      <c r="G25" s="60"/>
-      <c r="H25" s="60"/>
-      <c r="I25" s="60"/>
-      <c r="J25" s="61"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="61"/>
+      <c r="F25" s="61"/>
+      <c r="G25" s="61"/>
+      <c r="H25" s="61"/>
+      <c r="I25" s="61"/>
+      <c r="J25" s="62"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B26" s="58">
+      <c r="B26" s="52">
         <v>16</v>
       </c>
-      <c r="C26" s="40">
-        <v>512</v>
-      </c>
-      <c r="D26" s="41">
+      <c r="C26" s="34">
+        <v>512</v>
+      </c>
+      <c r="D26" s="35">
         <v>480</v>
       </c>
-      <c r="E26" s="41">
-        <v>512</v>
-      </c>
-      <c r="F26" s="41">
-        <v>128</v>
-      </c>
-      <c r="G26" s="41">
-        <v>32</v>
-      </c>
-      <c r="H26" s="50">
-        <v>32</v>
-      </c>
-      <c r="I26" s="46">
+      <c r="E26" s="35">
+        <v>512</v>
+      </c>
+      <c r="F26" s="35">
+        <v>128</v>
+      </c>
+      <c r="G26" s="35">
+        <v>32</v>
+      </c>
+      <c r="H26" s="44">
+        <v>32</v>
+      </c>
+      <c r="I26" s="40">
         <v>4.71</v>
       </c>
-      <c r="J26" s="45">
+      <c r="J26" s="39">
         <f t="shared" si="0"/>
         <v>0.20226954155672824</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B27" s="37">
+      <c r="B27" s="31">
         <v>17</v>
       </c>
-      <c r="C27" s="42">
+      <c r="C27" s="36">
         <v>1024</v>
       </c>
-      <c r="D27" s="33">
+      <c r="D27" s="27">
         <v>480</v>
       </c>
-      <c r="E27" s="33">
+      <c r="E27" s="27">
         <v>1024</v>
       </c>
-      <c r="F27" s="33">
-        <v>128</v>
-      </c>
-      <c r="G27" s="33">
-        <v>32</v>
-      </c>
-      <c r="H27" s="51">
-        <v>32</v>
-      </c>
-      <c r="I27" s="47">
+      <c r="F27" s="27">
+        <v>128</v>
+      </c>
+      <c r="G27" s="27">
+        <v>32</v>
+      </c>
+      <c r="H27" s="45">
+        <v>32</v>
+      </c>
+      <c r="I27" s="41">
         <v>10.26</v>
       </c>
-      <c r="J27" s="34">
+      <c r="J27" s="28">
         <f t="shared" si="0"/>
         <v>0.44061263192612138</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B28" s="37">
+      <c r="B28" s="31">
         <v>18</v>
       </c>
-      <c r="C28" s="42">
+      <c r="C28" s="36">
         <v>2048</v>
       </c>
-      <c r="D28" s="33">
+      <c r="D28" s="27">
         <v>480</v>
       </c>
-      <c r="E28" s="33">
+      <c r="E28" s="27">
         <v>2048</v>
       </c>
-      <c r="F28" s="33">
-        <v>128</v>
-      </c>
-      <c r="G28" s="33">
-        <v>32</v>
-      </c>
-      <c r="H28" s="51">
-        <v>32</v>
-      </c>
-      <c r="I28" s="47">
+      <c r="F28" s="27">
+        <v>128</v>
+      </c>
+      <c r="G28" s="27">
+        <v>32</v>
+      </c>
+      <c r="H28" s="45">
+        <v>32</v>
+      </c>
+      <c r="I28" s="41">
         <v>13.19</v>
       </c>
-      <c r="J28" s="34">
+      <c r="J28" s="28">
         <f t="shared" si="0"/>
         <v>0.56644060576077393</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B29" s="37">
+      <c r="B29" s="31">
         <v>19</v>
       </c>
-      <c r="C29" s="42">
+      <c r="C29" s="36">
         <v>4096</v>
       </c>
-      <c r="D29" s="33">
+      <c r="D29" s="27">
         <v>480</v>
       </c>
-      <c r="E29" s="33">
+      <c r="E29" s="27">
         <v>4096</v>
       </c>
-      <c r="F29" s="33">
-        <v>128</v>
-      </c>
-      <c r="G29" s="33">
-        <v>32</v>
-      </c>
-      <c r="H29" s="51">
-        <v>32</v>
-      </c>
-      <c r="I29" s="47">
+      <c r="F29" s="27">
+        <v>128</v>
+      </c>
+      <c r="G29" s="27">
+        <v>32</v>
+      </c>
+      <c r="H29" s="45">
+        <v>32</v>
+      </c>
+      <c r="I29" s="41">
         <v>14.83</v>
       </c>
-      <c r="J29" s="34">
+      <c r="J29" s="28">
         <f t="shared" si="0"/>
         <v>0.63686991534740545</v>
       </c>
     </row>
     <row r="30" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B30" s="38">
+      <c r="B30" s="32">
         <v>20</v>
       </c>
-      <c r="C30" s="43">
+      <c r="C30" s="37">
         <v>8192</v>
       </c>
-      <c r="D30" s="35">
+      <c r="D30" s="29">
         <v>480</v>
       </c>
-      <c r="E30" s="35">
+      <c r="E30" s="29">
         <v>8192</v>
       </c>
-      <c r="F30" s="35">
-        <v>128</v>
-      </c>
-      <c r="G30" s="35">
-        <v>32</v>
-      </c>
-      <c r="H30" s="52">
-        <v>32</v>
-      </c>
-      <c r="I30" s="48">
+      <c r="F30" s="29">
+        <v>128</v>
+      </c>
+      <c r="G30" s="29">
+        <v>32</v>
+      </c>
+      <c r="H30" s="46">
+        <v>32</v>
+      </c>
+      <c r="I30" s="42">
         <v>14.43</v>
       </c>
-      <c r="J30" s="36">
+      <c r="J30" s="30">
         <f t="shared" si="0"/>
         <v>0.61969203496042213</v>
       </c>
@@ -2380,4 +2384,760 @@
     <oddHeader>&amp;L&amp;"Arial"&amp;10&amp;K0078D7[AMD Official Use Only - Internal Distribution Only]&amp;1#</oddHeader>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA624FCB-E3F0-4C6F-AFE6-E77862410E78}">
+  <dimension ref="B3:J30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="16384" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B3" s="26"/>
+      <c r="C3" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="24">
+        <v>758</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="24">
+        <v>120</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="24">
+        <f>D3*512*F3/1000/1000</f>
+        <v>46.57152</v>
+      </c>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="26"/>
+    </row>
+    <row r="5" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="26"/>
+      <c r="C5" s="26"/>
+      <c r="D5" s="26"/>
+      <c r="E5" s="26"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="26"/>
+      <c r="J5" s="26"/>
+    </row>
+    <row r="6" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B6" s="51" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" s="47" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="60" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="61"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="61"/>
+      <c r="I7" s="61"/>
+      <c r="J7" s="62"/>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B8" s="48">
+        <v>1</v>
+      </c>
+      <c r="C8" s="34">
+        <v>512</v>
+      </c>
+      <c r="D8" s="35">
+        <v>512</v>
+      </c>
+      <c r="E8" s="35">
+        <v>512</v>
+      </c>
+      <c r="F8" s="35">
+        <v>32</v>
+      </c>
+      <c r="G8" s="35">
+        <v>128</v>
+      </c>
+      <c r="H8" s="44">
+        <v>64</v>
+      </c>
+      <c r="I8" s="40">
+        <v>6.17</v>
+      </c>
+      <c r="J8" s="39">
+        <f>I8/$H$3</f>
+        <v>0.13248440248460863</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B9" s="49">
+        <v>2</v>
+      </c>
+      <c r="C9" s="36">
+        <v>512</v>
+      </c>
+      <c r="D9" s="27">
+        <v>1024</v>
+      </c>
+      <c r="E9" s="27">
+        <v>1024</v>
+      </c>
+      <c r="F9" s="27">
+        <v>32</v>
+      </c>
+      <c r="G9" s="27">
+        <v>128</v>
+      </c>
+      <c r="H9" s="45">
+        <v>64</v>
+      </c>
+      <c r="I9" s="41">
+        <v>11.54</v>
+      </c>
+      <c r="J9" s="28">
+        <f t="shared" ref="J9:J30" si="0">I9/$H$3</f>
+        <v>0.24779092458223392</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B10" s="49">
+        <v>3</v>
+      </c>
+      <c r="C10" s="36">
+        <v>512</v>
+      </c>
+      <c r="D10" s="27">
+        <v>2048</v>
+      </c>
+      <c r="E10" s="27">
+        <v>2048</v>
+      </c>
+      <c r="F10" s="27">
+        <v>32</v>
+      </c>
+      <c r="G10" s="27">
+        <v>128</v>
+      </c>
+      <c r="H10" s="45">
+        <v>64</v>
+      </c>
+      <c r="I10" s="41">
+        <v>19.45</v>
+      </c>
+      <c r="J10" s="28">
+        <f t="shared" si="0"/>
+        <v>0.41763721690853123</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B11" s="49">
+        <v>4</v>
+      </c>
+      <c r="C11" s="36">
+        <v>512</v>
+      </c>
+      <c r="D11" s="27">
+        <v>4096</v>
+      </c>
+      <c r="E11" s="27">
+        <v>4096</v>
+      </c>
+      <c r="F11" s="27">
+        <v>32</v>
+      </c>
+      <c r="G11" s="27">
+        <v>128</v>
+      </c>
+      <c r="H11" s="45">
+        <v>64</v>
+      </c>
+      <c r="I11" s="41">
+        <v>25.3</v>
+      </c>
+      <c r="J11" s="28">
+        <f t="shared" si="0"/>
+        <v>0.54325046723834658</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="50">
+        <v>5</v>
+      </c>
+      <c r="C12" s="37">
+        <v>512</v>
+      </c>
+      <c r="D12" s="29">
+        <v>8192</v>
+      </c>
+      <c r="E12" s="29">
+        <v>8192</v>
+      </c>
+      <c r="F12" s="29">
+        <v>32</v>
+      </c>
+      <c r="G12" s="29">
+        <v>128</v>
+      </c>
+      <c r="H12" s="46">
+        <v>64</v>
+      </c>
+      <c r="I12" s="42">
+        <v>29.48</v>
+      </c>
+      <c r="J12" s="30">
+        <f t="shared" si="0"/>
+        <v>0.63300489226033418</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="60" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="61"/>
+      <c r="D13" s="61"/>
+      <c r="E13" s="61"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="61"/>
+      <c r="H13" s="61"/>
+      <c r="I13" s="61"/>
+      <c r="J13" s="62"/>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B14" s="48">
+        <v>6</v>
+      </c>
+      <c r="C14" s="34">
+        <v>512</v>
+      </c>
+      <c r="D14" s="35">
+        <v>512</v>
+      </c>
+      <c r="E14" s="35">
+        <v>512</v>
+      </c>
+      <c r="F14" s="35">
+        <v>128</v>
+      </c>
+      <c r="G14" s="35">
+        <v>32</v>
+      </c>
+      <c r="H14" s="44">
+        <v>64</v>
+      </c>
+      <c r="I14" s="40">
+        <v>6.1</v>
+      </c>
+      <c r="J14" s="39">
+        <f t="shared" si="0"/>
+        <v>0.13098133795074757</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B15" s="49">
+        <v>7</v>
+      </c>
+      <c r="C15" s="36">
+        <v>1024</v>
+      </c>
+      <c r="D15" s="27">
+        <v>512</v>
+      </c>
+      <c r="E15" s="27">
+        <v>1024</v>
+      </c>
+      <c r="F15" s="27">
+        <v>128</v>
+      </c>
+      <c r="G15" s="27">
+        <v>32</v>
+      </c>
+      <c r="H15" s="45">
+        <v>64</v>
+      </c>
+      <c r="I15" s="41">
+        <v>11.44</v>
+      </c>
+      <c r="J15" s="28">
+        <f t="shared" si="0"/>
+        <v>0.24564368953386104</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B16" s="49">
+        <v>8</v>
+      </c>
+      <c r="C16" s="36">
+        <v>2048</v>
+      </c>
+      <c r="D16" s="27">
+        <v>512</v>
+      </c>
+      <c r="E16" s="27">
+        <v>2048</v>
+      </c>
+      <c r="F16" s="27">
+        <v>128</v>
+      </c>
+      <c r="G16" s="27">
+        <v>32</v>
+      </c>
+      <c r="H16" s="45">
+        <v>64</v>
+      </c>
+      <c r="I16" s="41">
+        <v>20.399999999999999</v>
+      </c>
+      <c r="J16" s="28">
+        <f t="shared" si="0"/>
+        <v>0.43803594986807387</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B17" s="49">
+        <v>9</v>
+      </c>
+      <c r="C17" s="36">
+        <v>4096</v>
+      </c>
+      <c r="D17" s="27">
+        <v>512</v>
+      </c>
+      <c r="E17" s="27">
+        <v>4096</v>
+      </c>
+      <c r="F17" s="27">
+        <v>128</v>
+      </c>
+      <c r="G17" s="27">
+        <v>32</v>
+      </c>
+      <c r="H17" s="45">
+        <v>64</v>
+      </c>
+      <c r="I17" s="41">
+        <v>25.82</v>
+      </c>
+      <c r="J17" s="28">
+        <f t="shared" si="0"/>
+        <v>0.55441608948988563</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="50">
+        <v>10</v>
+      </c>
+      <c r="C18" s="37">
+        <v>8192</v>
+      </c>
+      <c r="D18" s="29">
+        <v>512</v>
+      </c>
+      <c r="E18" s="29">
+        <v>8192</v>
+      </c>
+      <c r="F18" s="29">
+        <v>128</v>
+      </c>
+      <c r="G18" s="29">
+        <v>32</v>
+      </c>
+      <c r="H18" s="46">
+        <v>64</v>
+      </c>
+      <c r="I18" s="42">
+        <v>24.05</v>
+      </c>
+      <c r="J18" s="30">
+        <f t="shared" si="0"/>
+        <v>0.51641002913368517</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B19" s="60" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="61"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="61"/>
+      <c r="H19" s="61"/>
+      <c r="I19" s="61"/>
+      <c r="J19" s="62"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B20" s="48">
+        <v>11</v>
+      </c>
+      <c r="C20" s="34">
+        <v>480</v>
+      </c>
+      <c r="D20" s="35">
+        <v>512</v>
+      </c>
+      <c r="E20" s="35">
+        <v>512</v>
+      </c>
+      <c r="F20" s="35">
+        <v>32</v>
+      </c>
+      <c r="G20" s="35">
+        <v>128</v>
+      </c>
+      <c r="H20" s="44">
+        <v>64</v>
+      </c>
+      <c r="I20" s="40">
+        <v>5.6</v>
+      </c>
+      <c r="J20" s="39">
+        <f t="shared" si="0"/>
+        <v>0.12024516270888302</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B21" s="49">
+        <v>12</v>
+      </c>
+      <c r="C21" s="36">
+        <v>480</v>
+      </c>
+      <c r="D21" s="27">
+        <v>1024</v>
+      </c>
+      <c r="E21" s="27">
+        <v>1024</v>
+      </c>
+      <c r="F21" s="27">
+        <v>32</v>
+      </c>
+      <c r="G21" s="27">
+        <v>128</v>
+      </c>
+      <c r="H21" s="45">
+        <v>64</v>
+      </c>
+      <c r="I21" s="41">
+        <v>14.12</v>
+      </c>
+      <c r="J21" s="28">
+        <f t="shared" si="0"/>
+        <v>0.30318958883025504</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B22" s="49">
+        <v>13</v>
+      </c>
+      <c r="C22" s="36">
+        <v>480</v>
+      </c>
+      <c r="D22" s="27">
+        <v>2048</v>
+      </c>
+      <c r="E22" s="27">
+        <v>2048</v>
+      </c>
+      <c r="F22" s="27">
+        <v>32</v>
+      </c>
+      <c r="G22" s="27">
+        <v>128</v>
+      </c>
+      <c r="H22" s="45">
+        <v>64</v>
+      </c>
+      <c r="I22" s="41">
+        <v>23.32</v>
+      </c>
+      <c r="J22" s="28">
+        <f t="shared" si="0"/>
+        <v>0.50073521328056292</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B23" s="49">
+        <v>14</v>
+      </c>
+      <c r="C23" s="36">
+        <v>480</v>
+      </c>
+      <c r="D23" s="27">
+        <v>4096</v>
+      </c>
+      <c r="E23" s="27">
+        <v>4096</v>
+      </c>
+      <c r="F23" s="27">
+        <v>32</v>
+      </c>
+      <c r="G23" s="27">
+        <v>128</v>
+      </c>
+      <c r="H23" s="45">
+        <v>64</v>
+      </c>
+      <c r="I23" s="41">
+        <v>27.28</v>
+      </c>
+      <c r="J23" s="28">
+        <f t="shared" si="0"/>
+        <v>0.58576572119613024</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B24" s="50">
+        <v>15</v>
+      </c>
+      <c r="C24" s="37">
+        <v>480</v>
+      </c>
+      <c r="D24" s="29">
+        <v>8192</v>
+      </c>
+      <c r="E24" s="29">
+        <v>8192</v>
+      </c>
+      <c r="F24" s="29">
+        <v>32</v>
+      </c>
+      <c r="G24" s="29">
+        <v>128</v>
+      </c>
+      <c r="H24" s="46">
+        <v>64</v>
+      </c>
+      <c r="I24" s="42">
+        <v>30</v>
+      </c>
+      <c r="J24" s="30">
+        <f t="shared" si="0"/>
+        <v>0.64417051451187335</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B25" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" s="61"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="61"/>
+      <c r="F25" s="61"/>
+      <c r="G25" s="61"/>
+      <c r="H25" s="61"/>
+      <c r="I25" s="61"/>
+      <c r="J25" s="62"/>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B26" s="52">
+        <v>16</v>
+      </c>
+      <c r="C26" s="34">
+        <v>512</v>
+      </c>
+      <c r="D26" s="35">
+        <v>480</v>
+      </c>
+      <c r="E26" s="35">
+        <v>512</v>
+      </c>
+      <c r="F26" s="35">
+        <v>128</v>
+      </c>
+      <c r="G26" s="35">
+        <v>32</v>
+      </c>
+      <c r="H26" s="44">
+        <v>64</v>
+      </c>
+      <c r="I26" s="40">
+        <v>5.85</v>
+      </c>
+      <c r="J26" s="39">
+        <f t="shared" si="0"/>
+        <v>0.1256132503298153</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B27" s="31">
+        <v>17</v>
+      </c>
+      <c r="C27" s="36">
+        <v>1024</v>
+      </c>
+      <c r="D27" s="27">
+        <v>480</v>
+      </c>
+      <c r="E27" s="27">
+        <v>1024</v>
+      </c>
+      <c r="F27" s="27">
+        <v>128</v>
+      </c>
+      <c r="G27" s="27">
+        <v>32</v>
+      </c>
+      <c r="H27" s="45">
+        <v>64</v>
+      </c>
+      <c r="I27" s="41">
+        <v>15</v>
+      </c>
+      <c r="J27" s="28">
+        <f t="shared" si="0"/>
+        <v>0.32208525725593667</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B28" s="31">
+        <v>18</v>
+      </c>
+      <c r="C28" s="36">
+        <v>2048</v>
+      </c>
+      <c r="D28" s="27">
+        <v>480</v>
+      </c>
+      <c r="E28" s="27">
+        <v>2048</v>
+      </c>
+      <c r="F28" s="27">
+        <v>128</v>
+      </c>
+      <c r="G28" s="27">
+        <v>32</v>
+      </c>
+      <c r="H28" s="45">
+        <v>64</v>
+      </c>
+      <c r="I28" s="41">
+        <v>24.22</v>
+      </c>
+      <c r="J28" s="28">
+        <f t="shared" si="0"/>
+        <v>0.52006032871591912</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B29" s="31">
+        <v>19</v>
+      </c>
+      <c r="C29" s="36">
+        <v>4096</v>
+      </c>
+      <c r="D29" s="27">
+        <v>480</v>
+      </c>
+      <c r="E29" s="27">
+        <v>4096</v>
+      </c>
+      <c r="F29" s="27">
+        <v>128</v>
+      </c>
+      <c r="G29" s="27">
+        <v>32</v>
+      </c>
+      <c r="H29" s="45">
+        <v>64</v>
+      </c>
+      <c r="I29" s="41">
+        <v>27.72</v>
+      </c>
+      <c r="J29" s="28">
+        <f t="shared" si="0"/>
+        <v>0.59521355540897092</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B30" s="32">
+        <v>20</v>
+      </c>
+      <c r="C30" s="37">
+        <v>8192</v>
+      </c>
+      <c r="D30" s="29">
+        <v>480</v>
+      </c>
+      <c r="E30" s="29">
+        <v>8192</v>
+      </c>
+      <c r="F30" s="29">
+        <v>128</v>
+      </c>
+      <c r="G30" s="29">
+        <v>32</v>
+      </c>
+      <c r="H30" s="46">
+        <v>64</v>
+      </c>
+      <c r="I30" s="42">
+        <v>24.8</v>
+      </c>
+      <c r="J30" s="30">
+        <f t="shared" si="0"/>
+        <v>0.53251429199648204</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="B7:J7"/>
+    <mergeCell ref="B13:J13"/>
+    <mergeCell ref="B19:J19"/>
+    <mergeCell ref="B25:J25"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"Arial"&amp;10&amp;K0078D7[AMD Official Use Only - Internal Distribution Only]&amp;1#</oddHeader>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
bf16 1K size perf align with rpk
</commit_message>
<xml_diff>
--- a/doc/性能.xlsx
+++ b/doc/性能.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feiw\source\repos\TensileLite\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFAB5739-094C-43D1-8F93-5FFCA431942D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EF86F7-52DC-41B9-AED1-FC3805D83CBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-12645" windowWidth="16440" windowHeight="28440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -108,7 +108,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -163,6 +163,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="31">
     <border>
@@ -584,7 +590,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -770,6 +776,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2390,8 +2399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA624FCB-E3F0-4C6F-AFE6-E77862410E78}">
   <dimension ref="B3:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2844,7 +2853,7 @@
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B21" s="49">
+      <c r="B21" s="63">
         <v>12</v>
       </c>
       <c r="C21" s="36">

</xml_diff>

<commit_message>
opt loop for 960*1k 64*128*32 for bf16
</commit_message>
<xml_diff>
--- a/doc/性能.xlsx
+++ b/doc/性能.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feiw\source\repos\TensileLite\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9EF86F7-52DC-41B9-AED1-FC3805D83CBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535140FE-F449-4CBB-9948-20284DF669E2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-16320" yWindow="-12645" windowWidth="16440" windowHeight="28440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -590,7 +590,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -748,6 +748,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -778,7 +781,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1064,7 +1067,7 @@
   <dimension ref="B4:N12"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:XFD1048576"/>
+      <selection activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1094,18 +1097,18 @@
         <f>D5*1024*F5/1000</f>
         <v>93143.039999999994</v>
       </c>
-      <c r="I5" s="53" t="s">
+      <c r="I5" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="54"/>
-      <c r="K5" s="55">
+      <c r="J5" s="55"/>
+      <c r="K5" s="56">
         <v>43885</v>
       </c>
-      <c r="L5" s="56"/>
-      <c r="M5" s="57">
+      <c r="L5" s="57"/>
+      <c r="M5" s="58">
         <v>43889</v>
       </c>
-      <c r="N5" s="58"/>
+      <c r="N5" s="59"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
@@ -1384,18 +1387,18 @@
         <f>D5*1024*F5/1000</f>
         <v>93143.039999999994</v>
       </c>
-      <c r="I5" s="53" t="s">
+      <c r="I5" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="54"/>
-      <c r="K5" s="55">
+      <c r="J5" s="55"/>
+      <c r="K5" s="56">
         <v>43885</v>
       </c>
-      <c r="L5" s="56"/>
-      <c r="M5" s="57">
+      <c r="L5" s="57"/>
+      <c r="M5" s="58">
         <v>43889</v>
       </c>
-      <c r="N5" s="58"/>
+      <c r="N5" s="59"/>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.35">
       <c r="B6" s="7" t="s">
@@ -1673,8 +1676,8 @@
         <f>D3*256*F3/1000/1000</f>
         <v>23.28576</v>
       </c>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="25"/>
@@ -1728,17 +1731,17 @@
       </c>
     </row>
     <row r="7" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="60" t="s">
+      <c r="B7" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="61"/>
-      <c r="H7" s="61"/>
-      <c r="I7" s="61"/>
-      <c r="J7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="63"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="48">
@@ -1891,17 +1894,17 @@
       </c>
     </row>
     <row r="13" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="60" t="s">
+      <c r="B13" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="61"/>
-      <c r="H13" s="61"/>
-      <c r="I13" s="61"/>
-      <c r="J13" s="62"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="63"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="48">
@@ -2054,17 +2057,17 @@
       </c>
     </row>
     <row r="19" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="60" t="s">
+      <c r="B19" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="61"/>
-      <c r="D19" s="61"/>
-      <c r="E19" s="61"/>
-      <c r="F19" s="61"/>
-      <c r="G19" s="61"/>
-      <c r="H19" s="61"/>
-      <c r="I19" s="61"/>
-      <c r="J19" s="62"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="62"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="63"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B20" s="48">
@@ -2217,17 +2220,17 @@
       </c>
     </row>
     <row r="25" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="60" t="s">
+      <c r="B25" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="61"/>
-      <c r="D25" s="61"/>
-      <c r="E25" s="61"/>
-      <c r="F25" s="61"/>
-      <c r="G25" s="61"/>
-      <c r="H25" s="61"/>
-      <c r="I25" s="61"/>
-      <c r="J25" s="62"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="62"/>
+      <c r="G25" s="62"/>
+      <c r="H25" s="62"/>
+      <c r="I25" s="62"/>
+      <c r="J25" s="63"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B26" s="52">
@@ -2397,10 +2400,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA624FCB-E3F0-4C6F-AFE6-E77862410E78}">
-  <dimension ref="B3:J30"/>
+  <dimension ref="B2:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K33" sqref="K33"/>
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2408,13 +2411,18 @@
     <col min="1" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="D2" s="1">
+        <v>758</v>
+      </c>
+    </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B3" s="26"/>
       <c r="C3" s="24" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="24">
-        <v>758</v>
+        <v>1280</v>
       </c>
       <c r="E3" s="24" t="s">
         <v>2</v>
@@ -2427,10 +2435,10 @@
       </c>
       <c r="H3" s="24">
         <f>D3*512*F3/1000/1000</f>
-        <v>46.57152</v>
-      </c>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
+        <v>78.643199999999993</v>
+      </c>
+      <c r="I3" s="60"/>
+      <c r="J3" s="60"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B4" s="26"/>
@@ -2484,17 +2492,17 @@
       </c>
     </row>
     <row r="7" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B7" s="60" t="s">
+      <c r="B7" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="61"/>
-      <c r="F7" s="61"/>
-      <c r="G7" s="61"/>
-      <c r="H7" s="61"/>
-      <c r="I7" s="61"/>
-      <c r="J7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="63"/>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="48">
@@ -2523,7 +2531,7 @@
       </c>
       <c r="J8" s="39">
         <f>I8/$H$3</f>
-        <v>0.13248440248460863</v>
+        <v>7.8455607096354171E-2</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.35">
@@ -2552,8 +2560,8 @@
         <v>11.54</v>
       </c>
       <c r="J9" s="28">
-        <f t="shared" ref="J9:J30" si="0">I9/$H$3</f>
-        <v>0.24779092458223392</v>
+        <f t="shared" ref="J9:J32" si="0">I9/$H$3</f>
+        <v>0.14673868815104166</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.35">
@@ -2583,7 +2591,7 @@
       </c>
       <c r="J10" s="28">
         <f t="shared" si="0"/>
-        <v>0.41763721690853123</v>
+        <v>0.24731953938802084</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.35">
@@ -2613,7 +2621,7 @@
       </c>
       <c r="J11" s="28">
         <f t="shared" si="0"/>
-        <v>0.54325046723834658</v>
+        <v>0.32170613606770837</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2643,21 +2651,21 @@
       </c>
       <c r="J12" s="30">
         <f t="shared" si="0"/>
-        <v>0.63300489226033418</v>
+        <v>0.37485758463541669</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="60" t="s">
+      <c r="B13" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="61"/>
-      <c r="F13" s="61"/>
-      <c r="G13" s="61"/>
-      <c r="H13" s="61"/>
-      <c r="I13" s="61"/>
-      <c r="J13" s="62"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="62"/>
+      <c r="F13" s="62"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="62"/>
+      <c r="J13" s="63"/>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" s="48">
@@ -2686,7 +2694,7 @@
       </c>
       <c r="J14" s="39">
         <f t="shared" si="0"/>
-        <v>0.13098133795074757</v>
+        <v>7.7565511067708329E-2</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.35">
@@ -2716,7 +2724,7 @@
       </c>
       <c r="J15" s="28">
         <f t="shared" si="0"/>
-        <v>0.24564368953386104</v>
+        <v>0.14546712239583334</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.35">
@@ -2746,7 +2754,7 @@
       </c>
       <c r="J16" s="28">
         <f t="shared" si="0"/>
-        <v>0.43803594986807387</v>
+        <v>0.2593994140625</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.35">
@@ -2776,7 +2784,7 @@
       </c>
       <c r="J17" s="28">
         <f t="shared" si="0"/>
-        <v>0.55441608948988563</v>
+        <v>0.32831827799479169</v>
       </c>
     </row>
     <row r="18" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2806,21 +2814,21 @@
       </c>
       <c r="J18" s="30">
         <f t="shared" si="0"/>
-        <v>0.51641002913368517</v>
+        <v>0.30581156412760419</v>
       </c>
     </row>
     <row r="19" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="60" t="s">
+      <c r="B19" s="61" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="61"/>
-      <c r="D19" s="61"/>
-      <c r="E19" s="61"/>
-      <c r="F19" s="61"/>
-      <c r="G19" s="61"/>
-      <c r="H19" s="61"/>
-      <c r="I19" s="61"/>
-      <c r="J19" s="62"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="62"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="63"/>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B20" s="48">
@@ -2849,11 +2857,11 @@
       </c>
       <c r="J20" s="39">
         <f t="shared" si="0"/>
-        <v>0.12024516270888302</v>
+        <v>7.1207682291666671E-2</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B21" s="63">
+      <c r="B21" s="53">
         <v>12</v>
       </c>
       <c r="C21" s="36">
@@ -2879,7 +2887,7 @@
       </c>
       <c r="J21" s="28">
         <f t="shared" si="0"/>
-        <v>0.30318958883025504</v>
+        <v>0.17954508463541669</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.35">
@@ -2909,7 +2917,7 @@
       </c>
       <c r="J22" s="28">
         <f t="shared" si="0"/>
-        <v>0.50073521328056292</v>
+        <v>0.29652913411458337</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.35">
@@ -2939,7 +2947,7 @@
       </c>
       <c r="J23" s="28">
         <f t="shared" si="0"/>
-        <v>0.58576572119613024</v>
+        <v>0.34688313802083337</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2969,21 +2977,21 @@
       </c>
       <c r="J24" s="30">
         <f t="shared" si="0"/>
-        <v>0.64417051451187335</v>
+        <v>0.38146972656250006</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B25" s="60" t="s">
+      <c r="B25" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="C25" s="61"/>
-      <c r="D25" s="61"/>
-      <c r="E25" s="61"/>
-      <c r="F25" s="61"/>
-      <c r="G25" s="61"/>
-      <c r="H25" s="61"/>
-      <c r="I25" s="61"/>
-      <c r="J25" s="62"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="62"/>
+      <c r="G25" s="62"/>
+      <c r="H25" s="62"/>
+      <c r="I25" s="62"/>
+      <c r="J25" s="63"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B26" s="52">
@@ -3012,7 +3020,7 @@
       </c>
       <c r="J26" s="39">
         <f t="shared" si="0"/>
-        <v>0.1256132503298153</v>
+        <v>7.43865966796875E-2</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.35">
@@ -3042,7 +3050,7 @@
       </c>
       <c r="J27" s="28">
         <f t="shared" si="0"/>
-        <v>0.32208525725593667</v>
+        <v>0.19073486328125003</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.35">
@@ -3072,7 +3080,7 @@
       </c>
       <c r="J28" s="28">
         <f t="shared" si="0"/>
-        <v>0.52006032871591912</v>
+        <v>0.30797322591145837</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.35">
@@ -3102,7 +3110,7 @@
       </c>
       <c r="J29" s="28">
         <f t="shared" si="0"/>
-        <v>0.59521355540897092</v>
+        <v>0.35247802734375</v>
       </c>
     </row>
     <row r="30" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -3132,7 +3140,16 @@
       </c>
       <c r="J30" s="30">
         <f t="shared" si="0"/>
-        <v>0.53251429199648204</v>
+        <v>0.31534830729166669</v>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="I32" s="1">
+        <v>55.430999999999997</v>
+      </c>
+      <c r="J32" s="64">
+        <f t="shared" si="0"/>
+        <v>0.70484161376953125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>